<commit_message>
ACX-32769: Update units_import_template.xlsx file
</commit_message>
<xml_diff>
--- a/apps/main/src/assets/templates/units_import_template.xlsx
+++ b/apps/main/src/assets/templates/units_import_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D23131C-9644-FE41-A780-7FE2F649067B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8669920-E919-B54F-A731-47216E39A562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="1180" windowWidth="28720" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The contact name for this unit. This is a mandatory field</t>
+          <t>This is a mandatory field</t>
         </r>
       </text>
     </comment>
@@ -128,7 +128,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The email for the contact on this unit. All email around tenant access and secret changes will be sent to this address.</t>
+          <t>Email of the resident. All email around tenant access and secret changes will be sent to this address.</t>
         </r>
       </text>
     </comment>
@@ -142,7 +142,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The phone number for the contact on this unit. Format +&lt;country code&gt;&lt;phone number&gt;</t>
+          <t>Phone number of the resident. Format +&lt;country code&gt;&lt;phone number&gt;</t>
         </r>
       </text>
     </comment>
@@ -171,10 +171,10 @@
     <t>Guest Vlan</t>
   </si>
   <si>
-    <t>Contact Name</t>
-  </si>
-  <si>
     <t>Unit Vlan</t>
+  </si>
+  <si>
+    <t>Resident Name</t>
   </si>
 </sst>
 </file>
@@ -269,9 +269,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -309,9 +309,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,26 +344,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,26 +379,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -592,7 +558,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -613,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -622,7 +588,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>

</xml_diff>